<commit_message>
added semantic search and changed request methods
</commit_message>
<xml_diff>
--- a/opensoft-autocomplete-results.xlsx
+++ b/opensoft-autocomplete-results.xlsx
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t xml:space="preserve">In Transit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">falsdk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falsk som vatten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One False Move</t>
   </si>
 </sst>
 </file>
@@ -511,6 +520,49 @@
         <v>35</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>68.29260699999577</v>
+      </c>
+      <c r="G3">
+        <v>0.16801000000123167</v>
+      </c>
+      <c r="H3">
+        <v>69.31573699999717</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: format of timestamp in watch history
</commit_message>
<xml_diff>
--- a/opensoft-autocomplete-results.xlsx
+++ b/opensoft-autocomplete-results.xlsx
@@ -131,6 +131,333 @@
   </si>
   <si>
     <t xml:space="preserve">One False Move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Italian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Black Pirate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Son of the Sheik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Broadway Melody</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Devil to Pay!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Champ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Front Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Crowd Roars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Barretts of Wimpole Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Gay Divorcee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Lost Patrol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twentieth Century</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The World Moves On</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Band Concert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three Ages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Thief of Bagdad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Itali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Italian Job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Italian Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piazza Fontana: The Italian Conspiracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Birds, the Bees and the Italians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italian for Beginners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italiano medio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marriage Italian Style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jealousy, Italian Style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An Italian Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emergency Exit: Young Italians Abroad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Imaginarium of Doctor Parnassus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mambo Italiano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Voyage to Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It Is Written in the Stars, Inspector Palmu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forget Baghdad: Jews and Arabs - The Iraqi Connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy: Love It, or Leave It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Thrill of It All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It Was the Son</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It Begins with the End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That's It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That's the Way I Like It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bring It On: In It to Win It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Knack... and How to Get It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Iron Horse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Invisible Ray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Informer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Inn of the Sixth Happiness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Incredible Shrinking Man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Innocents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Inheritance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ipcress File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Incident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Immortal Story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Inextinguishable Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Illustrated Man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Iceman Cometh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Illumination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Wedding March</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild and Woolly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Shadows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winsor McCay, the Famous Cartoonist of the N.Y. Herald and His Moving Comics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild Oranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westfront 1918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild Boys of the Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where Are My Children?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wonder Bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wife! Be Like a Rose!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Banners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who Killed Cock Robin?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waikiki Wedding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wuthering Heights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woman of the Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wonder Man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woman in a Dressing Gown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woodstock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Women in Love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would You Kill a Child?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Womanlight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wolfen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Women on the Verge of a Nervous Breakdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working Girl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Gone Wild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World of Glory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World War II: When Lions Roared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woyzeck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word of Honor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work Hard, Play Hard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Trade Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workingman's Death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wordplay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World War Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worlds Apart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World's Greatest Dad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Without End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Words and Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World of Tomorrow</t>
   </si>
 </sst>
 </file>
@@ -563,6 +890,929 @@
       <c r="W3"/>
       <c r="X3"/>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>141.50769999995828</v>
+      </c>
+      <c r="G4">
+        <v>0.12239999999292195</v>
+      </c>
+      <c r="H4">
+        <v>172.60939999995753</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" t="s">
+        <v>48</v>
+      </c>
+      <c r="S4" t="s">
+        <v>49</v>
+      </c>
+      <c r="T4" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V4" t="s">
+        <v>52</v>
+      </c>
+      <c r="W4" t="s">
+        <v>53</v>
+      </c>
+      <c r="X4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>100.98599999991711</v>
+      </c>
+      <c r="G5">
+        <v>0.07350000005681068</v>
+      </c>
+      <c r="H5">
+        <v>101.3061999999918</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>47</v>
+      </c>
+      <c r="R5" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" t="s">
+        <v>49</v>
+      </c>
+      <c r="T5" t="s">
+        <v>50</v>
+      </c>
+      <c r="U5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5" t="s">
+        <v>54</v>
+      </c>
+      <c r="W5" t="s">
+        <v>56</v>
+      </c>
+      <c r="X5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>314.72970000002533</v>
+      </c>
+      <c r="G6">
+        <v>0.09580000001005828</v>
+      </c>
+      <c r="H6">
+        <v>315.13440000009723</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6" t="s">
+        <v>62</v>
+      </c>
+      <c r="P6" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" t="s">
+        <v>65</v>
+      </c>
+      <c r="S6" t="s">
+        <v>66</v>
+      </c>
+      <c r="T6" t="s">
+        <v>67</v>
+      </c>
+      <c r="U6" t="s">
+        <v>68</v>
+      </c>
+      <c r="V6" t="s">
+        <v>69</v>
+      </c>
+      <c r="W6" t="s">
+        <v>70</v>
+      </c>
+      <c r="X6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>143.88000000000466</v>
+      </c>
+      <c r="G7">
+        <v>0.03539999993517995</v>
+      </c>
+      <c r="H7">
+        <v>144.09169999998994</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" t="s">
+        <v>61</v>
+      </c>
+      <c r="O7" t="s">
+        <v>62</v>
+      </c>
+      <c r="P7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R7" t="s">
+        <v>74</v>
+      </c>
+      <c r="S7" t="s">
+        <v>70</v>
+      </c>
+      <c r="T7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U7" t="s">
+        <v>75</v>
+      </c>
+      <c r="V7" t="s">
+        <v>76</v>
+      </c>
+      <c r="W7" t="s">
+        <v>77</v>
+      </c>
+      <c r="X7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>253.2053999999771</v>
+      </c>
+      <c r="G8">
+        <v>0.03029999998398125</v>
+      </c>
+      <c r="H8">
+        <v>253.32569999992847</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" t="s">
+        <v>79</v>
+      </c>
+      <c r="P8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>81</v>
+      </c>
+      <c r="R8" t="s">
+        <v>82</v>
+      </c>
+      <c r="S8" t="s">
+        <v>83</v>
+      </c>
+      <c r="T8" t="s">
+        <v>84</v>
+      </c>
+      <c r="U8" t="s">
+        <v>84</v>
+      </c>
+      <c r="V8" t="s">
+        <v>85</v>
+      </c>
+      <c r="W8" t="s">
+        <v>75</v>
+      </c>
+      <c r="X8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>105.9605000000447</v>
+      </c>
+      <c r="G9">
+        <v>0.036500000045634806</v>
+      </c>
+      <c r="H9">
+        <v>106.15579999994952</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" t="s">
+        <v>89</v>
+      </c>
+      <c r="M9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N9" t="s">
+        <v>91</v>
+      </c>
+      <c r="O9" t="s">
+        <v>92</v>
+      </c>
+      <c r="P9" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>94</v>
+      </c>
+      <c r="R9" t="s">
+        <v>95</v>
+      </c>
+      <c r="S9" t="s">
+        <v>96</v>
+      </c>
+      <c r="T9" t="s">
+        <v>97</v>
+      </c>
+      <c r="U9" t="s">
+        <v>98</v>
+      </c>
+      <c r="V9" t="s">
+        <v>99</v>
+      </c>
+      <c r="W9" t="s">
+        <v>100</v>
+      </c>
+      <c r="X9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>104.84070000005886</v>
+      </c>
+      <c r="G10">
+        <v>0.028400000068359077</v>
+      </c>
+      <c r="H10">
+        <v>104.94130000006407</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" t="s">
+        <v>45</v>
+      </c>
+      <c r="P10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>47</v>
+      </c>
+      <c r="R10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" t="s">
+        <v>49</v>
+      </c>
+      <c r="T10" t="s">
+        <v>50</v>
+      </c>
+      <c r="U10" t="s">
+        <v>53</v>
+      </c>
+      <c r="V10" t="s">
+        <v>54</v>
+      </c>
+      <c r="W10" t="s">
+        <v>57</v>
+      </c>
+      <c r="X10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>100.71440000005532</v>
+      </c>
+      <c r="G11">
+        <v>0.033300000010058284</v>
+      </c>
+      <c r="H11">
+        <v>100.830600000103</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" t="s">
+        <v>45</v>
+      </c>
+      <c r="P11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11" t="s">
+        <v>48</v>
+      </c>
+      <c r="S11" t="s">
+        <v>49</v>
+      </c>
+      <c r="T11" t="s">
+        <v>50</v>
+      </c>
+      <c r="U11" t="s">
+        <v>53</v>
+      </c>
+      <c r="V11" t="s">
+        <v>54</v>
+      </c>
+      <c r="W11" t="s">
+        <v>57</v>
+      </c>
+      <c r="X11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>99.02389999991283</v>
+      </c>
+      <c r="G12">
+        <v>0.05400000000372529</v>
+      </c>
+      <c r="H12">
+        <v>99.14709999994375</v>
+      </c>
+      <c r="J12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N12" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" t="s">
+        <v>45</v>
+      </c>
+      <c r="P12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" t="s">
+        <v>48</v>
+      </c>
+      <c r="S12" t="s">
+        <v>49</v>
+      </c>
+      <c r="T12" t="s">
+        <v>50</v>
+      </c>
+      <c r="U12" t="s">
+        <v>53</v>
+      </c>
+      <c r="V12" t="s">
+        <v>54</v>
+      </c>
+      <c r="W12" t="s">
+        <v>56</v>
+      </c>
+      <c r="X12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>10490.530000000028</v>
+      </c>
+      <c r="G13">
+        <v>0.025399999925866723</v>
+      </c>
+      <c r="H13">
+        <v>10490.639899999951</v>
+      </c>
+      <c r="J13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M13" t="s">
+        <v>60</v>
+      </c>
+      <c r="N13" t="s">
+        <v>61</v>
+      </c>
+      <c r="O13" t="s">
+        <v>62</v>
+      </c>
+      <c r="P13" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>74</v>
+      </c>
+      <c r="R13" t="s">
+        <v>63</v>
+      </c>
+      <c r="S13" t="s">
+        <v>73</v>
+      </c>
+      <c r="T13" t="s">
+        <v>77</v>
+      </c>
+      <c r="U13" t="s">
+        <v>64</v>
+      </c>
+      <c r="V13" t="s">
+        <v>65</v>
+      </c>
+      <c r="W13" t="s">
+        <v>66</v>
+      </c>
+      <c r="X13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>107.59840000001714</v>
+      </c>
+      <c r="G14">
+        <v>0.025999999954365194</v>
+      </c>
+      <c r="H14">
+        <v>107.79579999996349</v>
+      </c>
+      <c r="J14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K14" t="s">
+        <v>108</v>
+      </c>
+      <c r="L14" t="s">
+        <v>109</v>
+      </c>
+      <c r="M14" t="s">
+        <v>110</v>
+      </c>
+      <c r="N14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O14" t="s">
+        <v>112</v>
+      </c>
+      <c r="P14" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>114</v>
+      </c>
+      <c r="R14" t="s">
+        <v>115</v>
+      </c>
+      <c r="S14" t="s">
+        <v>116</v>
+      </c>
+      <c r="T14" t="s">
+        <v>117</v>
+      </c>
+      <c r="U14" t="s">
+        <v>118</v>
+      </c>
+      <c r="V14" t="s">
+        <v>119</v>
+      </c>
+      <c r="W14" t="s">
+        <v>120</v>
+      </c>
+      <c r="X14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>110.67779999994673</v>
+      </c>
+      <c r="G15">
+        <v>0.02370000001974404</v>
+      </c>
+      <c r="H15">
+        <v>110.81059999996796</v>
+      </c>
+      <c r="J15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K15" t="s">
+        <v>121</v>
+      </c>
+      <c r="L15" t="s">
+        <v>123</v>
+      </c>
+      <c r="M15" t="s">
+        <v>124</v>
+      </c>
+      <c r="N15" t="s">
+        <v>125</v>
+      </c>
+      <c r="O15" t="s">
+        <v>126</v>
+      </c>
+      <c r="P15" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>128</v>
+      </c>
+      <c r="R15" t="s">
+        <v>129</v>
+      </c>
+      <c r="S15" t="s">
+        <v>130</v>
+      </c>
+      <c r="T15" t="s">
+        <v>131</v>
+      </c>
+      <c r="U15" t="s">
+        <v>132</v>
+      </c>
+      <c r="V15" t="s">
+        <v>133</v>
+      </c>
+      <c r="W15" t="s">
+        <v>134</v>
+      </c>
+      <c r="X15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>145.21249999990687</v>
+      </c>
+      <c r="G16">
+        <v>0.0158000000519678</v>
+      </c>
+      <c r="H16">
+        <v>145.44200000003912</v>
+      </c>
+      <c r="J16" t="s">
+        <v>131</v>
+      </c>
+      <c r="K16" t="s">
+        <v>132</v>
+      </c>
+      <c r="L16" t="s">
+        <v>133</v>
+      </c>
+      <c r="M16" t="s">
+        <v>134</v>
+      </c>
+      <c r="N16" t="s">
+        <v>137</v>
+      </c>
+      <c r="O16" t="s">
+        <v>138</v>
+      </c>
+      <c r="P16" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>140</v>
+      </c>
+      <c r="R16" t="s">
+        <v>141</v>
+      </c>
+      <c r="S16" t="s">
+        <v>142</v>
+      </c>
+      <c r="T16" t="s">
+        <v>143</v>
+      </c>
+      <c r="U16" t="s">
+        <v>144</v>
+      </c>
+      <c r="V16" t="s">
+        <v>145</v>
+      </c>
+      <c r="W16" t="s">
+        <v>146</v>
+      </c>
+      <c r="X16" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
feat added openai embeddings and triggers
</commit_message>
<xml_diff>
--- a/opensoft-autocomplete-results.xlsx
+++ b/opensoft-autocomplete-results.xlsx
@@ -131,6 +131,438 @@
   </si>
   <si>
     <t xml:space="preserve">One False Move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Woman of Paris: A Drama of Fate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asphalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Free Soul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anna Karenina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alice Adams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Night at the Opera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angels with Dirty Faces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Midsummer Night's Dream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anthony Adverse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexander's Ragtime Band</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Man to Remember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arise, My Love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Damsel in Distress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angelina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Song to Remember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Streetcar Named Desire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Star Is Born</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Sun-Tribe Myth from the Bakumatsu Era</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Summer Place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Shot in the Dark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Swedish Love Story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Slave of Love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Summer at Grandpa's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Sunday in the Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Soldier's Story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Soldier's Tale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Shock to the System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a so</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Soldier's Daughter Never Cries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Soldier's Sweetheart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Song for Martin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Somewhat Gentle Man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Echoes From a Somber Empire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Father of a Soldier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So Much So Fast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With a Song in My Heart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurt Cobain About a Son</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I Want to Be a Soldier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Touch the Sound: A Sound Journey with Evelyn Glennie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a son</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of a Lion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of a Gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Earth Is a Sinful Song</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Song for a Raggy Boy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son frère</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harry &amp; Son</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Native Son</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesus' Son</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Son</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Son</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Son</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild and Woolly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Shadows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winsor McCay, the Famous Cartoonist of the N.Y. Herald and His Moving Comics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild Oranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westfront 1918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild Boys of the Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where Are My Children?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wonder Bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wife! Be Like a Rose!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Banners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who Killed Cock Robin?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waikiki Wedding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wuthering Heights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woman of the Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Without Pity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winchester '73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild Love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Witness for the Prosecution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will Success Spoil Rock Hunter?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild River</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winnetou: The Last Shot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winnetou: The Red Gentleman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winnetou and Old Firehand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winnie the Pooh and the Honey Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winnie the Pooh and Tigger Too</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windwalker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winners &amp; Sinners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wings of Desire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Window to Paris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winter Sleepers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind with the Gone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">winj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lady Windermere's Fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children in the Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gone with the Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Hen in the Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Winslow Boy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rear Window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inherit the Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any Number Can Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">winjs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Young Winston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scorching Winds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everybody Wins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Wings of the Dove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wings of Hope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broken Wings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Times and Winds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secret of the Wings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When Pigs Have Wings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">winjsw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The House of the Laughing Windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">winjswe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upstream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Under Capricorn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ugetsu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Under Ten Flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un uomo da bruciare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une Femme Marièe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up the Down Staircase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ulysses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukroshcheniye ognya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ugly, Dirty and Bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un uomo in ginocchio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uppercut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un papillon sur l'èpaule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno sceriffo extraterrestre... poco extra e molto terrestre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used Cars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bringing Up Baby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strike Up the Band</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murderers Among Us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give Us This Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Set-Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somebody Up There Likes Me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paris Belongs to Us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seven Up!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Round-Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Come Have Coffee with Us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Michele aveva un gallo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schoolgirls Growing Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's Up, Doc?</t>
   </si>
 </sst>
 </file>
@@ -563,6 +995,1735 @@
       <c r="W3"/>
       <c r="X3"/>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>422.0330740000063</v>
+      </c>
+      <c r="G4">
+        <v>0.1505489999835845</v>
+      </c>
+      <c r="H4">
+        <v>422.4901499999978</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" t="s">
+        <v>48</v>
+      </c>
+      <c r="S4" t="s">
+        <v>49</v>
+      </c>
+      <c r="T4" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V4" t="s">
+        <v>52</v>
+      </c>
+      <c r="W4" t="s">
+        <v>53</v>
+      </c>
+      <c r="X4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>57.374780999991344</v>
+      </c>
+      <c r="G5">
+        <v>0.07150900000124238</v>
+      </c>
+      <c r="H5">
+        <v>57.546504999976605</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>47</v>
+      </c>
+      <c r="R5" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" t="s">
+        <v>49</v>
+      </c>
+      <c r="T5" t="s">
+        <v>50</v>
+      </c>
+      <c r="U5" t="s">
+        <v>51</v>
+      </c>
+      <c r="V5" t="s">
+        <v>52</v>
+      </c>
+      <c r="W5" t="s">
+        <v>53</v>
+      </c>
+      <c r="X5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>351.042277999979</v>
+      </c>
+      <c r="G6">
+        <v>0.02546000000438653</v>
+      </c>
+      <c r="H6">
+        <v>351.3864159999939</v>
+      </c>
+      <c r="J6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" t="s">
+        <v>61</v>
+      </c>
+      <c r="P6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T6" t="s">
+        <v>57</v>
+      </c>
+      <c r="U6" t="s">
+        <v>65</v>
+      </c>
+      <c r="V6" t="s">
+        <v>66</v>
+      </c>
+      <c r="W6" t="s">
+        <v>67</v>
+      </c>
+      <c r="X6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>281.9260490000015</v>
+      </c>
+      <c r="G7">
+        <v>0.07489099999656901</v>
+      </c>
+      <c r="H7">
+        <v>282.1788210000086</v>
+      </c>
+      <c r="J7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" t="s">
+        <v>71</v>
+      </c>
+      <c r="O7" t="s">
+        <v>72</v>
+      </c>
+      <c r="P7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R7" t="s">
+        <v>75</v>
+      </c>
+      <c r="S7" t="s">
+        <v>75</v>
+      </c>
+      <c r="T7" t="s">
+        <v>76</v>
+      </c>
+      <c r="U7" t="s">
+        <v>77</v>
+      </c>
+      <c r="V7" t="s">
+        <v>78</v>
+      </c>
+      <c r="W7" t="s">
+        <v>79</v>
+      </c>
+      <c r="X7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>126.02052399999229</v>
+      </c>
+      <c r="G8">
+        <v>0.06671799998730421</v>
+      </c>
+      <c r="H8">
+        <v>126.24349400002393</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" t="s">
+        <v>72</v>
+      </c>
+      <c r="L8" t="s">
+        <v>78</v>
+      </c>
+      <c r="M8" t="s">
+        <v>82</v>
+      </c>
+      <c r="N8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O8" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>85</v>
+      </c>
+      <c r="R8" t="s">
+        <v>86</v>
+      </c>
+      <c r="S8" t="s">
+        <v>87</v>
+      </c>
+      <c r="T8" t="s">
+        <v>88</v>
+      </c>
+      <c r="U8" t="s">
+        <v>89</v>
+      </c>
+      <c r="V8" t="s">
+        <v>90</v>
+      </c>
+      <c r="W8" t="s">
+        <v>91</v>
+      </c>
+      <c r="X8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>171.46267800001078</v>
+      </c>
+      <c r="G9">
+        <v>0.0349819999828469</v>
+      </c>
+      <c r="H9">
+        <v>171.76165600001696</v>
+      </c>
+      <c r="J9" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" t="s">
+        <v>71</v>
+      </c>
+      <c r="O9" t="s">
+        <v>72</v>
+      </c>
+      <c r="P9" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>74</v>
+      </c>
+      <c r="R9" t="s">
+        <v>75</v>
+      </c>
+      <c r="S9" t="s">
+        <v>75</v>
+      </c>
+      <c r="T9" t="s">
+        <v>76</v>
+      </c>
+      <c r="U9" t="s">
+        <v>77</v>
+      </c>
+      <c r="V9" t="s">
+        <v>78</v>
+      </c>
+      <c r="W9" t="s">
+        <v>79</v>
+      </c>
+      <c r="X9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>76.48554900000454</v>
+      </c>
+      <c r="G10">
+        <v>0.03410799999255687</v>
+      </c>
+      <c r="H10">
+        <v>76.69802300000447</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" t="s">
+        <v>59</v>
+      </c>
+      <c r="N10" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" t="s">
+        <v>61</v>
+      </c>
+      <c r="P10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>63</v>
+      </c>
+      <c r="R10" t="s">
+        <v>58</v>
+      </c>
+      <c r="S10" t="s">
+        <v>64</v>
+      </c>
+      <c r="T10" t="s">
+        <v>57</v>
+      </c>
+      <c r="U10" t="s">
+        <v>65</v>
+      </c>
+      <c r="V10" t="s">
+        <v>66</v>
+      </c>
+      <c r="W10" t="s">
+        <v>67</v>
+      </c>
+      <c r="X10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>107.76829000000726</v>
+      </c>
+      <c r="G11">
+        <v>0.05197299999417737</v>
+      </c>
+      <c r="H11">
+        <v>107.92973400000483</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" t="s">
+        <v>45</v>
+      </c>
+      <c r="P11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11" t="s">
+        <v>48</v>
+      </c>
+      <c r="S11" t="s">
+        <v>49</v>
+      </c>
+      <c r="T11" t="s">
+        <v>50</v>
+      </c>
+      <c r="U11" t="s">
+        <v>51</v>
+      </c>
+      <c r="V11" t="s">
+        <v>52</v>
+      </c>
+      <c r="W11" t="s">
+        <v>53</v>
+      </c>
+      <c r="X11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>135.510037</v>
+      </c>
+      <c r="G12">
+        <v>0.05383900000015274</v>
+      </c>
+      <c r="H12">
+        <v>135.71059199998854</v>
+      </c>
+      <c r="J12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N12" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" t="s">
+        <v>45</v>
+      </c>
+      <c r="P12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" t="s">
+        <v>48</v>
+      </c>
+      <c r="S12" t="s">
+        <v>49</v>
+      </c>
+      <c r="T12" t="s">
+        <v>50</v>
+      </c>
+      <c r="U12" t="s">
+        <v>51</v>
+      </c>
+      <c r="V12" t="s">
+        <v>52</v>
+      </c>
+      <c r="W12" t="s">
+        <v>53</v>
+      </c>
+      <c r="X12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>68.86923999999999</v>
+      </c>
+      <c r="G13">
+        <v>0.06352500000502914</v>
+      </c>
+      <c r="H13">
+        <v>69.12036999998963</v>
+      </c>
+      <c r="J13" t="s">
+        <v>94</v>
+      </c>
+      <c r="K13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L13" t="s">
+        <v>96</v>
+      </c>
+      <c r="M13" t="s">
+        <v>97</v>
+      </c>
+      <c r="N13" t="s">
+        <v>98</v>
+      </c>
+      <c r="O13" t="s">
+        <v>99</v>
+      </c>
+      <c r="P13" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>101</v>
+      </c>
+      <c r="R13" t="s">
+        <v>102</v>
+      </c>
+      <c r="S13" t="s">
+        <v>103</v>
+      </c>
+      <c r="T13" t="s">
+        <v>104</v>
+      </c>
+      <c r="U13" t="s">
+        <v>105</v>
+      </c>
+      <c r="V13" t="s">
+        <v>106</v>
+      </c>
+      <c r="W13" t="s">
+        <v>107</v>
+      </c>
+      <c r="X13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>199.85483699999168</v>
+      </c>
+      <c r="G14">
+        <v>0.04905099997995421</v>
+      </c>
+      <c r="H14">
+        <v>200.23638200000278</v>
+      </c>
+      <c r="J14" t="s">
+        <v>94</v>
+      </c>
+      <c r="K14" t="s">
+        <v>96</v>
+      </c>
+      <c r="L14" t="s">
+        <v>97</v>
+      </c>
+      <c r="M14" t="s">
+        <v>98</v>
+      </c>
+      <c r="N14" t="s">
+        <v>100</v>
+      </c>
+      <c r="O14" t="s">
+        <v>103</v>
+      </c>
+      <c r="P14" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>111</v>
+      </c>
+      <c r="R14" t="s">
+        <v>77</v>
+      </c>
+      <c r="S14" t="s">
+        <v>112</v>
+      </c>
+      <c r="T14" t="s">
+        <v>113</v>
+      </c>
+      <c r="U14" t="s">
+        <v>114</v>
+      </c>
+      <c r="V14" t="s">
+        <v>115</v>
+      </c>
+      <c r="W14" t="s">
+        <v>116</v>
+      </c>
+      <c r="X14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>133.65385299999616</v>
+      </c>
+      <c r="G15">
+        <v>0.04455299998517148</v>
+      </c>
+      <c r="H15">
+        <v>133.97326299999258</v>
+      </c>
+      <c r="J15" t="s">
+        <v>96</v>
+      </c>
+      <c r="K15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L15" t="s">
+        <v>111</v>
+      </c>
+      <c r="M15" t="s">
+        <v>117</v>
+      </c>
+      <c r="N15" t="s">
+        <v>119</v>
+      </c>
+      <c r="O15" t="s">
+        <v>120</v>
+      </c>
+      <c r="P15" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>122</v>
+      </c>
+      <c r="R15" t="s">
+        <v>123</v>
+      </c>
+      <c r="S15" t="s">
+        <v>124</v>
+      </c>
+      <c r="T15" t="s">
+        <v>125</v>
+      </c>
+      <c r="U15" t="s">
+        <v>126</v>
+      </c>
+      <c r="V15" t="s">
+        <v>127</v>
+      </c>
+      <c r="W15" t="s">
+        <v>128</v>
+      </c>
+      <c r="X15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16"/>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>98.07760400002007</v>
+      </c>
+      <c r="G16">
+        <v>0.06080800000927411</v>
+      </c>
+      <c r="H16">
+        <v>98.29458600000362</v>
+      </c>
+      <c r="J16" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L16" t="s">
+        <v>96</v>
+      </c>
+      <c r="M16" t="s">
+        <v>132</v>
+      </c>
+      <c r="N16" t="s">
+        <v>133</v>
+      </c>
+      <c r="O16" t="s">
+        <v>134</v>
+      </c>
+      <c r="P16" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>136</v>
+      </c>
+      <c r="R16" t="s">
+        <v>111</v>
+      </c>
+      <c r="S16" t="s">
+        <v>137</v>
+      </c>
+      <c r="T16" t="s">
+        <v>138</v>
+      </c>
+      <c r="U16" t="s">
+        <v>139</v>
+      </c>
+      <c r="V16" t="s">
+        <v>119</v>
+      </c>
+      <c r="W16" t="s">
+        <v>117</v>
+      </c>
+      <c r="X16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17"/>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>107.30397000000812</v>
+      </c>
+      <c r="G17">
+        <v>0.038837999978568405</v>
+      </c>
+      <c r="H17">
+        <v>107.49626200000057</v>
+      </c>
+      <c r="J17" t="s">
+        <v>97</v>
+      </c>
+      <c r="K17" t="s">
+        <v>96</v>
+      </c>
+      <c r="L17" t="s">
+        <v>135</v>
+      </c>
+      <c r="M17" t="s">
+        <v>141</v>
+      </c>
+      <c r="N17" t="s">
+        <v>142</v>
+      </c>
+      <c r="O17" t="s">
+        <v>126</v>
+      </c>
+      <c r="P17" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>144</v>
+      </c>
+      <c r="R17" t="s">
+        <v>135</v>
+      </c>
+      <c r="S17" t="s">
+        <v>145</v>
+      </c>
+      <c r="T17" t="s">
+        <v>97</v>
+      </c>
+      <c r="U17" t="s">
+        <v>146</v>
+      </c>
+      <c r="V17" t="s">
+        <v>147</v>
+      </c>
+      <c r="W17" t="s">
+        <v>148</v>
+      </c>
+      <c r="X17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <v>185.85338899999624</v>
+      </c>
+      <c r="G18">
+        <v>0.038693000038620085</v>
+      </c>
+      <c r="H18">
+        <v>186.06535900000017</v>
+      </c>
+      <c r="J18" t="s">
+        <v>97</v>
+      </c>
+      <c r="K18" t="s">
+        <v>96</v>
+      </c>
+      <c r="L18" t="s">
+        <v>135</v>
+      </c>
+      <c r="M18" t="s">
+        <v>136</v>
+      </c>
+      <c r="N18" t="s">
+        <v>137</v>
+      </c>
+      <c r="O18" t="s">
+        <v>141</v>
+      </c>
+      <c r="P18" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>151</v>
+      </c>
+      <c r="R18" t="s">
+        <v>123</v>
+      </c>
+      <c r="S18" t="s">
+        <v>124</v>
+      </c>
+      <c r="T18" t="s">
+        <v>126</v>
+      </c>
+      <c r="U18" t="s">
+        <v>143</v>
+      </c>
+      <c r="V18" t="s">
+        <v>127</v>
+      </c>
+      <c r="W18" t="s">
+        <v>144</v>
+      </c>
+      <c r="X18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19"/>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>227.99944099999266</v>
+      </c>
+      <c r="G19">
+        <v>0.006050999974831939</v>
+      </c>
+      <c r="H19">
+        <v>228.13806399999885</v>
+      </c>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20"/>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+      <c r="F20">
+        <v>100.67128100001719</v>
+      </c>
+      <c r="G20">
+        <v>0.03993699996499345</v>
+      </c>
+      <c r="H20">
+        <v>100.95435200002976</v>
+      </c>
+      <c r="J20" t="s">
+        <v>97</v>
+      </c>
+      <c r="K20" t="s">
+        <v>96</v>
+      </c>
+      <c r="L20" t="s">
+        <v>135</v>
+      </c>
+      <c r="M20" t="s">
+        <v>136</v>
+      </c>
+      <c r="N20" t="s">
+        <v>137</v>
+      </c>
+      <c r="O20" t="s">
+        <v>141</v>
+      </c>
+      <c r="P20" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>151</v>
+      </c>
+      <c r="R20" t="s">
+        <v>123</v>
+      </c>
+      <c r="S20" t="s">
+        <v>124</v>
+      </c>
+      <c r="T20" t="s">
+        <v>126</v>
+      </c>
+      <c r="U20" t="s">
+        <v>143</v>
+      </c>
+      <c r="V20" t="s">
+        <v>127</v>
+      </c>
+      <c r="W20" t="s">
+        <v>144</v>
+      </c>
+      <c r="X20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21"/>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>15</v>
+      </c>
+      <c r="F21">
+        <v>96.62483899999643</v>
+      </c>
+      <c r="G21">
+        <v>0.04113099997630343</v>
+      </c>
+      <c r="H21">
+        <v>96.76025799999479</v>
+      </c>
+      <c r="J21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K21" t="s">
+        <v>96</v>
+      </c>
+      <c r="L21" t="s">
+        <v>135</v>
+      </c>
+      <c r="M21" t="s">
+        <v>141</v>
+      </c>
+      <c r="N21" t="s">
+        <v>142</v>
+      </c>
+      <c r="O21" t="s">
+        <v>126</v>
+      </c>
+      <c r="P21" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>144</v>
+      </c>
+      <c r="R21" t="s">
+        <v>135</v>
+      </c>
+      <c r="S21" t="s">
+        <v>145</v>
+      </c>
+      <c r="T21" t="s">
+        <v>97</v>
+      </c>
+      <c r="U21" t="s">
+        <v>146</v>
+      </c>
+      <c r="V21" t="s">
+        <v>147</v>
+      </c>
+      <c r="W21" t="s">
+        <v>148</v>
+      </c>
+      <c r="X21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>15</v>
+      </c>
+      <c r="F22">
+        <v>101.57776399998693</v>
+      </c>
+      <c r="G22">
+        <v>0.03659100004006177</v>
+      </c>
+      <c r="H22">
+        <v>101.70533800002886</v>
+      </c>
+      <c r="J22" t="s">
+        <v>97</v>
+      </c>
+      <c r="K22" t="s">
+        <v>131</v>
+      </c>
+      <c r="L22" t="s">
+        <v>96</v>
+      </c>
+      <c r="M22" t="s">
+        <v>132</v>
+      </c>
+      <c r="N22" t="s">
+        <v>133</v>
+      </c>
+      <c r="O22" t="s">
+        <v>134</v>
+      </c>
+      <c r="P22" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>136</v>
+      </c>
+      <c r="R22" t="s">
+        <v>111</v>
+      </c>
+      <c r="S22" t="s">
+        <v>137</v>
+      </c>
+      <c r="T22" t="s">
+        <v>138</v>
+      </c>
+      <c r="U22" t="s">
+        <v>139</v>
+      </c>
+      <c r="V22" t="s">
+        <v>119</v>
+      </c>
+      <c r="W22" t="s">
+        <v>117</v>
+      </c>
+      <c r="X22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+      <c r="F23">
+        <v>110.78586499998346</v>
+      </c>
+      <c r="G23">
+        <v>0.03984899999340996</v>
+      </c>
+      <c r="H23">
+        <v>110.99589700001525</v>
+      </c>
+      <c r="J23" t="s">
+        <v>96</v>
+      </c>
+      <c r="K23" t="s">
+        <v>97</v>
+      </c>
+      <c r="L23" t="s">
+        <v>111</v>
+      </c>
+      <c r="M23" t="s">
+        <v>117</v>
+      </c>
+      <c r="N23" t="s">
+        <v>119</v>
+      </c>
+      <c r="O23" t="s">
+        <v>120</v>
+      </c>
+      <c r="P23" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>122</v>
+      </c>
+      <c r="R23" t="s">
+        <v>123</v>
+      </c>
+      <c r="S23" t="s">
+        <v>124</v>
+      </c>
+      <c r="T23" t="s">
+        <v>125</v>
+      </c>
+      <c r="U23" t="s">
+        <v>126</v>
+      </c>
+      <c r="V23" t="s">
+        <v>127</v>
+      </c>
+      <c r="W23" t="s">
+        <v>128</v>
+      </c>
+      <c r="X23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <v>56.069550000014715</v>
+      </c>
+      <c r="G24">
+        <v>0.03622499998891726</v>
+      </c>
+      <c r="H24">
+        <v>56.21839100000216</v>
+      </c>
+      <c r="J24" t="s">
+        <v>94</v>
+      </c>
+      <c r="K24" t="s">
+        <v>96</v>
+      </c>
+      <c r="L24" t="s">
+        <v>97</v>
+      </c>
+      <c r="M24" t="s">
+        <v>98</v>
+      </c>
+      <c r="N24" t="s">
+        <v>100</v>
+      </c>
+      <c r="O24" t="s">
+        <v>103</v>
+      </c>
+      <c r="P24" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>111</v>
+      </c>
+      <c r="R24" t="s">
+        <v>77</v>
+      </c>
+      <c r="S24" t="s">
+        <v>112</v>
+      </c>
+      <c r="T24" t="s">
+        <v>113</v>
+      </c>
+      <c r="U24" t="s">
+        <v>114</v>
+      </c>
+      <c r="V24" t="s">
+        <v>115</v>
+      </c>
+      <c r="W24" t="s">
+        <v>116</v>
+      </c>
+      <c r="X24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>52.362787000020035</v>
+      </c>
+      <c r="G25">
+        <v>0.05497200001263991</v>
+      </c>
+      <c r="H25">
+        <v>52.68861000001198</v>
+      </c>
+      <c r="J25" t="s">
+        <v>94</v>
+      </c>
+      <c r="K25" t="s">
+        <v>95</v>
+      </c>
+      <c r="L25" t="s">
+        <v>96</v>
+      </c>
+      <c r="M25" t="s">
+        <v>97</v>
+      </c>
+      <c r="N25" t="s">
+        <v>98</v>
+      </c>
+      <c r="O25" t="s">
+        <v>99</v>
+      </c>
+      <c r="P25" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>101</v>
+      </c>
+      <c r="R25" t="s">
+        <v>102</v>
+      </c>
+      <c r="S25" t="s">
+        <v>103</v>
+      </c>
+      <c r="T25" t="s">
+        <v>104</v>
+      </c>
+      <c r="U25" t="s">
+        <v>105</v>
+      </c>
+      <c r="V25" t="s">
+        <v>106</v>
+      </c>
+      <c r="W25" t="s">
+        <v>107</v>
+      </c>
+      <c r="X25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>15</v>
+      </c>
+      <c r="F26">
+        <v>160.581223999965</v>
+      </c>
+      <c r="G26">
+        <v>0.04188899998553097</v>
+      </c>
+      <c r="H26">
+        <v>160.76832699996885</v>
+      </c>
+      <c r="J26" t="s">
+        <v>154</v>
+      </c>
+      <c r="K26" t="s">
+        <v>155</v>
+      </c>
+      <c r="L26" t="s">
+        <v>156</v>
+      </c>
+      <c r="M26" t="s">
+        <v>157</v>
+      </c>
+      <c r="N26" t="s">
+        <v>158</v>
+      </c>
+      <c r="O26" t="s">
+        <v>159</v>
+      </c>
+      <c r="P26" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>161</v>
+      </c>
+      <c r="R26" t="s">
+        <v>162</v>
+      </c>
+      <c r="S26" t="s">
+        <v>163</v>
+      </c>
+      <c r="T26" t="s">
+        <v>164</v>
+      </c>
+      <c r="U26" t="s">
+        <v>165</v>
+      </c>
+      <c r="V26" t="s">
+        <v>166</v>
+      </c>
+      <c r="W26" t="s">
+        <v>167</v>
+      </c>
+      <c r="X26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27"/>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>15</v>
+      </c>
+      <c r="E27">
+        <v>15</v>
+      </c>
+      <c r="F27">
+        <v>95.78993600001559</v>
+      </c>
+      <c r="G27">
+        <v>0.034882000007200986</v>
+      </c>
+      <c r="H27">
+        <v>95.95001799997408</v>
+      </c>
+      <c r="J27" t="s">
+        <v>170</v>
+      </c>
+      <c r="K27" t="s">
+        <v>171</v>
+      </c>
+      <c r="L27" t="s">
+        <v>172</v>
+      </c>
+      <c r="M27" t="s">
+        <v>173</v>
+      </c>
+      <c r="N27" t="s">
+        <v>174</v>
+      </c>
+      <c r="O27" t="s">
+        <v>175</v>
+      </c>
+      <c r="P27" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>158</v>
+      </c>
+      <c r="R27" t="s">
+        <v>177</v>
+      </c>
+      <c r="S27" t="s">
+        <v>178</v>
+      </c>
+      <c r="T27" t="s">
+        <v>160</v>
+      </c>
+      <c r="U27" t="s">
+        <v>179</v>
+      </c>
+      <c r="V27" t="s">
+        <v>180</v>
+      </c>
+      <c r="W27" t="s">
+        <v>181</v>
+      </c>
+      <c r="X27" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <v>55.52223000000231</v>
+      </c>
+      <c r="G28">
+        <v>0.03857599996263161</v>
+      </c>
+      <c r="H28">
+        <v>55.61392000003252</v>
+      </c>
+      <c r="J28" t="s">
+        <v>154</v>
+      </c>
+      <c r="K28" t="s">
+        <v>155</v>
+      </c>
+      <c r="L28" t="s">
+        <v>156</v>
+      </c>
+      <c r="M28" t="s">
+        <v>157</v>
+      </c>
+      <c r="N28" t="s">
+        <v>158</v>
+      </c>
+      <c r="O28" t="s">
+        <v>159</v>
+      </c>
+      <c r="P28" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>161</v>
+      </c>
+      <c r="R28" t="s">
+        <v>162</v>
+      </c>
+      <c r="S28" t="s">
+        <v>163</v>
+      </c>
+      <c r="T28" t="s">
+        <v>164</v>
+      </c>
+      <c r="U28" t="s">
+        <v>165</v>
+      </c>
+      <c r="V28" t="s">
+        <v>166</v>
+      </c>
+      <c r="W28" t="s">
+        <v>167</v>
+      </c>
+      <c r="X28" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>